<commit_message>
added water supplementation analysis
</commit_message>
<xml_diff>
--- a/results/noca_day_binn_results.xlsx
+++ b/results/noca_day_binn_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="full_tukey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,18 +22,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="203">
-  <si>
-    <t xml:space="preserve"> contrast</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> estimate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> df</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="203">
+  <si>
+    <t xml:space="preserve">contrast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">df</t>
   </si>
   <si>
     <t xml:space="preserve">t.ratio</t>
@@ -45,7 +45,7 @@
     <t xml:space="preserve"> 1.lwma - 2.lwma</t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;.0001</t>
+    <t xml:space="preserve">  &lt;.0001</t>
   </si>
   <si>
     <t xml:space="preserve"> 1.lwma - 3.lwma</t>
@@ -704,12 +704,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -732,8 +728,8 @@
   </sheetPr>
   <dimension ref="A1:F191"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A148" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A161" activeCellId="0" sqref="A161"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -766,16 +762,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>-0.514549</v>
+        <v>-0.5359</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0.0617</v>
+        <v>0.0572</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>-8.34</v>
+        <v>-9.364</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>7</v>
@@ -786,16 +782,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>-0.659749</v>
+        <v>-0.75965</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.0608</v>
+        <v>0.0536</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>-10.859</v>
+        <v>-14.164</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>7</v>
@@ -806,19 +802,19 @@
         <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>-0.798718</v>
+        <v>-0.33297</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.0584</v>
+        <v>0.078</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>-13.673</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>7</v>
+        <v>-4.267</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.004</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,19 +822,19 @@
         <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>-0.428536</v>
+        <v>-0.38426</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.0627</v>
+        <v>0.1758</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>-6.836</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>7</v>
+        <v>-2.186</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.8074</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -846,16 +842,16 @@
         <v>11</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>-0.605961</v>
+        <v>-0.64418</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.0602</v>
+        <v>0.0596</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>-10.07</v>
+        <v>-10.804</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>7</v>
@@ -866,16 +862,16 @@
         <v>12</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>-0.930944</v>
+        <v>-0.70155</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0.0593</v>
+        <v>0.0552</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>-15.691</v>
+        <v>-12.706</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>7</v>
@@ -886,19 +882,19 @@
         <v>13</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>-0.361</v>
+        <v>-0.04177</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>0.0651</v>
+        <v>0.0659</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>-5.547</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>7</v>
+        <v>-0.634</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -906,19 +902,19 @@
         <v>14</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0.108796</v>
+        <v>0.25086</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0.0697</v>
+        <v>0.085</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1.561</v>
+        <v>2.95</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0.9916</v>
+        <v>0.2651</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -926,19 +922,19 @@
         <v>15</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0.295008</v>
+        <v>1.15883</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>0.0865</v>
+        <v>0.2652</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>3.41</v>
+        <v>4.369</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>0.0811</v>
+        <v>0.0026</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,16 +942,16 @@
         <v>16</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>3.552333</v>
+        <v>3.41546</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>0.3611</v>
+        <v>0.3365</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>9.839</v>
+        <v>10.151</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>7</v>
@@ -966,16 +962,16 @@
         <v>17</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>4.121002</v>
+        <v>3.65623</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>0.4373</v>
+        <v>0.3438</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>9.425</v>
+        <v>10.636</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>7</v>
@@ -986,19 +982,19 @@
         <v>18</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>-0.286587</v>
+        <v>-0.1309</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>0.093</v>
+        <v>0.092</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>-3.082</v>
+        <v>-1.423</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0.1954</v>
+        <v>0.9973</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,16 +1002,16 @@
         <v>19</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>3.552156</v>
+        <v>3.62046</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>0.3901</v>
+        <v>0.4478</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>9.106</v>
+        <v>8.084</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>7</v>
@@ -1026,19 +1022,19 @@
         <v>20</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>3.66144</v>
+        <v>5.01801</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>0.4098</v>
+        <v>1.0248</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>8.934</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>7</v>
+        <v>4.897</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.0003</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,16 +1042,16 @@
         <v>21</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>1.870909</v>
+        <v>1.77374</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>0.1681</v>
+        <v>0.1839</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>11.131</v>
+        <v>9.643</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>7</v>
@@ -1066,16 +1062,16 @@
         <v>22</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>2.808501</v>
+        <v>2.642</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>0.265</v>
+        <v>0.1923</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>10.597</v>
+        <v>13.739</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>7</v>
@@ -1086,16 +1082,16 @@
         <v>23</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>2.497266</v>
+        <v>1.93689</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0.2934</v>
+        <v>0.1624</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>8.51</v>
+        <v>11.928</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>7</v>
@@ -1106,16 +1102,16 @@
         <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>2.057292</v>
+        <v>2.77394</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>0.1761</v>
+        <v>0.2775</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>11.685</v>
+        <v>9.995</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>7</v>
@@ -1126,16 +1122,16 @@
         <v>25</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>2.744139</v>
+        <v>2.78335</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>0.2497</v>
+        <v>0.475</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>10.992</v>
+        <v>5.86</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>7</v>
@@ -1146,19 +1142,19 @@
         <v>26</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>-0.145199</v>
+        <v>-0.22375</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>0.0513</v>
+        <v>0.0386</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>-2.831</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>0.3393</v>
+        <v>-5.797</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,19 +1162,19 @@
         <v>27</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>-0.284169</v>
+        <v>0.20293</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>0.0485</v>
+        <v>0.0686</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>-5.858</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>7</v>
+        <v>2.959</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>0.2598</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,19 +1182,19 @@
         <v>28</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0.086013</v>
+        <v>0.15164</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>0.0536</v>
+        <v>0.1718</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>1.605</v>
+        <v>0.883</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>0.9884</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,19 +1202,19 @@
         <v>29</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>-0.091411</v>
+        <v>-0.10828</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>0.0506</v>
+        <v>0.0466</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>-1.806</v>
+        <v>-2.325</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>0.9601</v>
+        <v>0.7156</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,19 +1222,19 @@
         <v>30</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>-0.416395</v>
+        <v>-0.16565</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>0.0496</v>
+        <v>0.0408</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>-8.394</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>7</v>
+        <v>-4.064</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>0.0088</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,19 +1242,19 @@
         <v>31</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>0.15355</v>
+        <v>0.49413</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>0.0564</v>
+        <v>0.0544</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>2.725</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>0.413</v>
+        <v>9.088</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,16 +1262,16 @@
         <v>32</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>0.623345</v>
+        <v>0.78676</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>0.0617</v>
+        <v>0.0765</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>10.111</v>
+        <v>10.29</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>7</v>
@@ -1286,16 +1282,16 @@
         <v>33</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>0.809557</v>
+        <v>1.69473</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>0.0802</v>
+        <v>0.2626</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>10.1</v>
+        <v>6.454</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>7</v>
@@ -1306,16 +1302,16 @@
         <v>34</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>4.066882</v>
+        <v>3.95136</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>0.3596</v>
+        <v>0.3344</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>11.31</v>
+        <v>11.817</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>7</v>
@@ -1326,16 +1322,16 @@
         <v>35</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>4.635551</v>
+        <v>4.19213</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>0.436</v>
+        <v>0.3417</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>10.631</v>
+        <v>12.267</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>7</v>
@@ -1346,19 +1342,19 @@
         <v>36</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>0.227962</v>
+        <v>0.405</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>0.0871</v>
+        <v>0.0841</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>2.618</v>
+        <v>4.813</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>0.4936</v>
+        <v>0.0004</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1366,16 +1362,16 @@
         <v>37</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>4.066705</v>
+        <v>4.15635</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>0.3887</v>
+        <v>0.4463</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>10.461</v>
+        <v>9.313</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>7</v>
@@ -1386,16 +1382,16 @@
         <v>38</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>4.17599</v>
+        <v>5.55391</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>0.4086</v>
+        <v>1.0241</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>10.221</v>
+        <v>5.423</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>7</v>
@@ -1406,16 +1402,16 @@
         <v>39</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>2.385459</v>
+        <v>2.30963</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>0.1649</v>
+        <v>0.1801</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>14.466</v>
+        <v>12.822</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>7</v>
@@ -1426,16 +1422,16 @@
         <v>40</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>3.32305</v>
+        <v>3.1779</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>0.263</v>
+        <v>0.1887</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>12.634</v>
+        <v>16.845</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>7</v>
@@ -1446,16 +1442,16 @@
         <v>41</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>3.011815</v>
+        <v>2.47279</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>0.2916</v>
+        <v>0.1581</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>10.327</v>
+        <v>15.645</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>7</v>
@@ -1466,16 +1462,16 @@
         <v>42</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>2.571841</v>
+        <v>3.30983</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>0.173</v>
+        <v>0.275</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>14.864</v>
+        <v>12.035</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>7</v>
@@ -1486,16 +1482,16 @@
         <v>43</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>3.258688</v>
+        <v>3.31925</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>0.2475</v>
+        <v>0.4735</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>13.165</v>
+        <v>7.009</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>7</v>
@@ -1506,19 +1502,19 @@
         <v>44</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>-0.13897</v>
+        <v>0.42668</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>0.0473</v>
+        <v>0.0656</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>-2.938</v>
-      </c>
-      <c r="F39" s="0" t="n">
-        <v>0.2719</v>
+        <v>6.503</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1526,19 +1522,19 @@
         <v>45</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>0.231212</v>
+        <v>0.37539</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>0.0525</v>
+        <v>0.1706</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>4.405</v>
+        <v>2.2</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>0.0022</v>
+        <v>0.7989</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1546,19 +1542,19 @@
         <v>46</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>0.053788</v>
+        <v>0.11547</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>0.0495</v>
+        <v>0.0421</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>1.088</v>
+        <v>2.745</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>0.9999</v>
+        <v>0.3984</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,19 +1562,19 @@
         <v>47</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>-0.271195</v>
+        <v>0.0581</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>0.0484</v>
+        <v>0.0355</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>-5.601</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>7</v>
+        <v>1.635</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0.9858</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,16 +1582,16 @@
         <v>48</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>0.298749</v>
+        <v>0.71788</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>0.0553</v>
+        <v>0.0506</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>5.401</v>
+        <v>14.196</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>7</v>
@@ -1606,16 +1602,16 @@
         <v>49</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>0.768544</v>
+        <v>1.01051</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>0.0607</v>
+        <v>0.0738</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E44" s="0" t="n">
-        <v>12.66</v>
+        <v>13.692</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>7</v>
@@ -1626,16 +1622,16 @@
         <v>50</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>0.954757</v>
+        <v>1.91848</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>0.0794</v>
+        <v>0.2618</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>12.021</v>
+        <v>7.327</v>
       </c>
       <c r="F45" s="0" t="s">
         <v>7</v>
@@ -1646,16 +1642,16 @@
         <v>51</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>4.212082</v>
+        <v>4.17511</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>0.3594</v>
+        <v>0.3338</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>11.719</v>
+        <v>12.508</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>7</v>
@@ -1666,16 +1662,16 @@
         <v>52</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>4.780751</v>
+        <v>4.41588</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>0.4359</v>
+        <v>0.3412</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>10.967</v>
+        <v>12.944</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>7</v>
@@ -1686,19 +1682,19 @@
         <v>53</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>0.373162</v>
+        <v>0.62875</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>0.0864</v>
+        <v>0.0817</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>4.318</v>
-      </c>
-      <c r="F48" s="0" t="n">
-        <v>0.0032</v>
+        <v>7.693</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,16 +1702,16 @@
         <v>54</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>4.211905</v>
+        <v>4.38011</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>0.3886</v>
+        <v>0.4458</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>10.839</v>
+        <v>9.825</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>7</v>
@@ -1726,16 +1722,16 @@
         <v>55</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>4.321189</v>
+        <v>5.77766</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>0.4084</v>
+        <v>1.0239</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E50" s="0" t="n">
-        <v>10.581</v>
+        <v>5.643</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>7</v>
@@ -1746,16 +1742,16 @@
         <v>56</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>2.530658</v>
+        <v>2.53339</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>0.1645</v>
+        <v>0.179</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>15.38</v>
+        <v>14.151</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>7</v>
@@ -1766,16 +1762,16 @@
         <v>57</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>3.468249</v>
+        <v>3.40165</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>0.2628</v>
+        <v>0.1876</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>13.197</v>
+        <v>18.133</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>7</v>
@@ -1786,16 +1782,16 @@
         <v>58</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>3.157015</v>
+        <v>2.69654</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>0.2914</v>
+        <v>0.1568</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>10.833</v>
+        <v>17.198</v>
       </c>
       <c r="F53" s="0" t="s">
         <v>7</v>
@@ -1806,16 +1802,16 @@
         <v>59</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>2.717041</v>
+        <v>3.53358</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>0.1727</v>
+        <v>0.2743</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>15.733</v>
+        <v>12.883</v>
       </c>
       <c r="F54" s="0" t="s">
         <v>7</v>
@@ -1826,16 +1822,16 @@
         <v>60</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>3.403888</v>
+        <v>3.543</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>0.2473</v>
+        <v>0.4731</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>13.765</v>
+        <v>7.489</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>7</v>
@@ -1846,19 +1842,19 @@
         <v>61</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>0.370182</v>
+        <v>-0.05129</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>0.0498</v>
+        <v>0.1798</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E56" s="0" t="n">
-        <v>7.439</v>
-      </c>
-      <c r="F56" s="0" t="s">
-        <v>7</v>
+        <v>-0.285</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1866,19 +1862,19 @@
         <v>62</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>0.192758</v>
+        <v>-0.31121</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>0.0466</v>
+        <v>0.0706</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>4.141</v>
+        <v>-4.409</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>0.0066</v>
+        <v>0.0022</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1886,19 +1882,19 @@
         <v>63</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>-0.132226</v>
+        <v>-0.36858</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>0.0455</v>
+        <v>0.0669</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>-2.909</v>
-      </c>
-      <c r="F58" s="0" t="n">
-        <v>0.2894</v>
+        <v>-5.509</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1906,19 +1902,19 @@
         <v>64</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>0.437719</v>
+        <v>0.2912</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>0.0527</v>
+        <v>0.076</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>8.3</v>
-      </c>
-      <c r="F59" s="0" t="s">
-        <v>7</v>
+        <v>3.833</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>0.0206</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,16 +1922,16 @@
         <v>65</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>0.907514</v>
+        <v>0.58383</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>0.0584</v>
+        <v>0.0931</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>15.549</v>
+        <v>6.273</v>
       </c>
       <c r="F60" s="0" t="s">
         <v>7</v>
@@ -1946,16 +1942,16 @@
         <v>66</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>1.093726</v>
+        <v>1.4918</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>0.0777</v>
+        <v>0.2679</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>14.085</v>
+        <v>5.569</v>
       </c>
       <c r="F61" s="0" t="s">
         <v>7</v>
@@ -1966,16 +1962,16 @@
         <v>67</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>4.351051</v>
+        <v>3.74843</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>0.359</v>
+        <v>0.3386</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E62" s="0" t="n">
-        <v>12.118</v>
+        <v>11.071</v>
       </c>
       <c r="F62" s="0" t="s">
         <v>7</v>
@@ -1986,16 +1982,16 @@
         <v>68</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>4.91972</v>
+        <v>3.9892</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>0.4356</v>
+        <v>0.3458</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>11.294</v>
+        <v>11.535</v>
       </c>
       <c r="F63" s="0" t="s">
         <v>7</v>
@@ -2006,19 +2002,19 @@
         <v>69</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>0.512131</v>
+        <v>0.20207</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>0.0848</v>
+        <v>0.0995</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E64" s="0" t="n">
-        <v>6.039</v>
-      </c>
-      <c r="F64" s="0" t="s">
-        <v>7</v>
+        <v>2.031</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>0.8877</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,16 +2022,16 @@
         <v>70</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>4.350874</v>
+        <v>3.95343</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>0.3882</v>
+        <v>0.4494</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E65" s="0" t="n">
-        <v>11.207</v>
+        <v>8.797</v>
       </c>
       <c r="F65" s="0" t="s">
         <v>7</v>
@@ -2046,19 +2042,19 @@
         <v>71</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>4.460159</v>
+        <v>5.35098</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>0.4081</v>
+        <v>1.0255</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E66" s="0" t="n">
-        <v>10.93</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>7</v>
+        <v>5.218</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>0.0001</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,16 +2062,16 @@
         <v>72</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>2.669628</v>
+        <v>2.1067</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>0.1637</v>
+        <v>0.1878</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E67" s="0" t="n">
-        <v>16.308</v>
+        <v>11.219</v>
       </c>
       <c r="F67" s="0" t="s">
         <v>7</v>
@@ -2086,16 +2082,16 @@
         <v>73</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>3.607219</v>
+        <v>2.97497</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>0.2623</v>
+        <v>0.196</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E68" s="0" t="n">
-        <v>13.754</v>
+        <v>15.18</v>
       </c>
       <c r="F68" s="0" t="s">
         <v>7</v>
@@ -2106,16 +2102,16 @@
         <v>74</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>3.295984</v>
+        <v>2.26986</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>0.291</v>
+        <v>0.1667</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E69" s="0" t="n">
-        <v>11.328</v>
+        <v>13.614</v>
       </c>
       <c r="F69" s="0" t="s">
         <v>7</v>
@@ -2126,16 +2122,16 @@
         <v>75</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>2.85601</v>
+        <v>3.1069</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>0.1719</v>
+        <v>0.2801</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E70" s="0" t="n">
-        <v>16.616</v>
+        <v>11.093</v>
       </c>
       <c r="F70" s="0" t="s">
         <v>7</v>
@@ -2146,16 +2142,16 @@
         <v>76</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>3.542857</v>
+        <v>3.11632</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>0.2467</v>
+        <v>0.4765</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E71" s="0" t="n">
-        <v>14.359</v>
+        <v>6.54</v>
       </c>
       <c r="F71" s="0" t="s">
         <v>7</v>
@@ -2166,19 +2162,19 @@
         <v>77</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>-0.177424</v>
+        <v>-0.25992</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>0.0518</v>
+        <v>0.1726</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E72" s="0" t="n">
-        <v>-3.424</v>
+        <v>-1.506</v>
       </c>
       <c r="F72" s="0" t="n">
-        <v>0.0778</v>
+        <v>0.9945</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2186,19 +2182,19 @@
         <v>78</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>-0.502408</v>
+        <v>-0.31729</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>0.0508</v>
+        <v>0.1711</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E73" s="0" t="n">
-        <v>-9.884</v>
-      </c>
-      <c r="F73" s="0" t="s">
-        <v>7</v>
+        <v>-1.854</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>0.9489</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2206,19 +2202,19 @@
         <v>79</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>0.067537</v>
+        <v>0.34249</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>0.0574</v>
+        <v>0.1749</v>
       </c>
       <c r="D74" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E74" s="0" t="n">
-        <v>1.176</v>
+        <v>1.958</v>
       </c>
       <c r="F74" s="0" t="n">
-        <v>0.9998</v>
+        <v>0.9169</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2226,19 +2222,19 @@
         <v>80</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>0.537332</v>
+        <v>0.63512</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>0.0626</v>
+        <v>0.183</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E75" s="0" t="n">
-        <v>8.578</v>
-      </c>
-      <c r="F75" s="0" t="s">
-        <v>7</v>
+        <v>3.471</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>0.0675</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2246,19 +2242,19 @@
         <v>81</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>0.723544</v>
+        <v>1.54309</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>0.0809</v>
+        <v>0.3108</v>
       </c>
       <c r="D76" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E76" s="0" t="n">
-        <v>8.942</v>
-      </c>
-      <c r="F76" s="0" t="s">
-        <v>7</v>
+        <v>4.965</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>0.0002</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2266,16 +2262,16 @@
         <v>82</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>3.980869</v>
+        <v>3.79972</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>0.3598</v>
+        <v>0.3734</v>
       </c>
       <c r="D77" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E77" s="0" t="n">
-        <v>11.065</v>
+        <v>10.176</v>
       </c>
       <c r="F77" s="0" t="s">
         <v>7</v>
@@ -2286,16 +2282,16 @@
         <v>83</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>4.549538</v>
+        <v>4.04049</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>0.4362</v>
+        <v>0.38</v>
       </c>
       <c r="D78" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E78" s="0" t="n">
-        <v>10.43</v>
+        <v>10.632</v>
       </c>
       <c r="F78" s="0" t="s">
         <v>7</v>
@@ -2306,19 +2302,19 @@
         <v>84</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>0.141949</v>
+        <v>0.25336</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>0.0878</v>
+        <v>0.1863</v>
       </c>
       <c r="D79" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E79" s="0" t="n">
-        <v>1.617</v>
+        <v>1.36</v>
       </c>
       <c r="F79" s="0" t="n">
-        <v>0.9874</v>
+        <v>0.9985</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2326,16 +2322,16 @@
         <v>85</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>3.980692</v>
+        <v>4.00472</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>0.3889</v>
+        <v>0.4762</v>
       </c>
       <c r="D80" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E80" s="0" t="n">
-        <v>10.236</v>
+        <v>8.409</v>
       </c>
       <c r="F80" s="0" t="s">
         <v>7</v>
@@ -2346,19 +2342,19 @@
         <v>86</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>4.089977</v>
+        <v>5.40227</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>0.4087</v>
+        <v>1.0375</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E81" s="0" t="n">
-        <v>10.007</v>
-      </c>
-      <c r="F81" s="0" t="s">
-        <v>7</v>
+        <v>5.207</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>0.0001</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2366,16 +2362,16 @@
         <v>87</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>2.299446</v>
+        <v>2.158</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>0.1653</v>
+        <v>0.2451</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E82" s="0" t="n">
-        <v>13.913</v>
+        <v>8.804</v>
       </c>
       <c r="F82" s="0" t="s">
         <v>7</v>
@@ -2386,16 +2382,16 @@
         <v>88</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>3.237037</v>
+        <v>3.02626</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>0.2633</v>
+        <v>0.2514</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E83" s="0" t="n">
-        <v>12.296</v>
+        <v>12.036</v>
       </c>
       <c r="F83" s="0" t="s">
         <v>7</v>
@@ -2406,16 +2402,16 @@
         <v>89</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>2.925802</v>
+        <v>2.32115</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>0.2918</v>
+        <v>0.2294</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E84" s="0" t="n">
-        <v>10.025</v>
+        <v>10.12</v>
       </c>
       <c r="F84" s="0" t="s">
         <v>7</v>
@@ -2426,16 +2422,16 @@
         <v>90</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>2.485828</v>
+        <v>3.1582</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>0.1734</v>
+        <v>0.3213</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E85" s="0" t="n">
-        <v>14.337</v>
+        <v>9.828</v>
       </c>
       <c r="F85" s="0" t="s">
         <v>7</v>
@@ -2446,16 +2442,16 @@
         <v>91</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>3.172675</v>
+        <v>3.16761</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>0.2478</v>
+        <v>0.5019</v>
       </c>
       <c r="D86" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E86" s="0" t="n">
-        <v>12.805</v>
+        <v>6.312</v>
       </c>
       <c r="F86" s="0" t="s">
         <v>7</v>
@@ -2466,19 +2462,19 @@
         <v>92</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>-0.324984</v>
+        <v>-0.05737</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>0.0477</v>
+        <v>0.0441</v>
       </c>
       <c r="D87" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E87" s="0" t="n">
-        <v>-6.814</v>
-      </c>
-      <c r="F87" s="0" t="s">
-        <v>7</v>
+        <v>-1.302</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <v>0.9991</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2486,19 +2482,19 @@
         <v>93</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>0.244961</v>
+        <v>0.60241</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>0.0547</v>
+        <v>0.0569</v>
       </c>
       <c r="D88" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E88" s="0" t="n">
-        <v>4.48</v>
-      </c>
-      <c r="F88" s="0" t="n">
-        <v>0.0016</v>
+        <v>10.59</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,16 +2502,16 @@
         <v>94</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>0.714756</v>
+        <v>0.89504</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>0.0601</v>
+        <v>0.0783</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E89" s="0" t="n">
-        <v>11.888</v>
+        <v>11.436</v>
       </c>
       <c r="F89" s="0" t="s">
         <v>7</v>
@@ -2526,16 +2522,16 @@
         <v>95</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>0.900969</v>
+        <v>1.80301</v>
       </c>
       <c r="C90" s="0" t="n">
-        <v>0.079</v>
+        <v>0.2631</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E90" s="0" t="n">
-        <v>11.407</v>
+        <v>6.852</v>
       </c>
       <c r="F90" s="0" t="s">
         <v>7</v>
@@ -2546,16 +2542,16 @@
         <v>96</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>4.158294</v>
+        <v>4.05964</v>
       </c>
       <c r="C91" s="0" t="n">
-        <v>0.3593</v>
+        <v>0.3348</v>
       </c>
       <c r="D91" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E91" s="0" t="n">
-        <v>11.572</v>
+        <v>12.125</v>
       </c>
       <c r="F91" s="0" t="s">
         <v>7</v>
@@ -2566,16 +2562,16 @@
         <v>97</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>4.726963</v>
+        <v>4.30041</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>0.4358</v>
+        <v>0.3422</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E92" s="0" t="n">
-        <v>10.846</v>
+        <v>12.569</v>
       </c>
       <c r="F92" s="0" t="s">
         <v>7</v>
@@ -2586,19 +2582,19 @@
         <v>98</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>0.319374</v>
+        <v>0.51328</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>0.086</v>
+        <v>0.0858</v>
       </c>
       <c r="D93" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E93" s="0" t="n">
-        <v>3.713</v>
-      </c>
-      <c r="F93" s="0" t="n">
-        <v>0.0311</v>
+        <v>5.983</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2606,16 +2602,16 @@
         <v>99</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>4.158117</v>
+        <v>4.26464</v>
       </c>
       <c r="C94" s="0" t="n">
-        <v>0.3885</v>
+        <v>0.4466</v>
       </c>
       <c r="D94" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E94" s="0" t="n">
-        <v>10.703</v>
+        <v>9.549</v>
       </c>
       <c r="F94" s="0" t="s">
         <v>7</v>
@@ -2626,16 +2622,16 @@
         <v>100</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>4.267401</v>
+        <v>5.66219</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>0.4083</v>
+        <v>1.0242</v>
       </c>
       <c r="D95" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E95" s="0" t="n">
-        <v>10.451</v>
+        <v>5.528</v>
       </c>
       <c r="F95" s="0" t="s">
         <v>7</v>
@@ -2646,16 +2642,16 @@
         <v>101</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>2.47687</v>
+        <v>2.41792</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>0.1643</v>
+        <v>0.1809</v>
       </c>
       <c r="D96" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E96" s="0" t="n">
-        <v>15.072</v>
+        <v>13.365</v>
       </c>
       <c r="F96" s="0" t="s">
         <v>7</v>
@@ -2666,16 +2662,16 @@
         <v>102</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>3.414461</v>
+        <v>3.28618</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>0.2627</v>
+        <v>0.1894</v>
       </c>
       <c r="D97" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E97" s="0" t="n">
-        <v>12.999</v>
+        <v>17.351</v>
       </c>
       <c r="F97" s="0" t="s">
         <v>7</v>
@@ -2686,16 +2682,16 @@
         <v>103</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>3.103227</v>
+        <v>2.58107</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>0.2913</v>
+        <v>0.1589</v>
       </c>
       <c r="D98" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E98" s="0" t="n">
-        <v>10.652</v>
+        <v>16.239</v>
       </c>
       <c r="F98" s="0" t="s">
         <v>7</v>
@@ -2706,16 +2702,16 @@
         <v>104</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>2.663253</v>
+        <v>3.41812</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>0.1725</v>
+        <v>0.2755</v>
       </c>
       <c r="D99" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E99" s="0" t="n">
-        <v>15.44</v>
+        <v>12.406</v>
       </c>
       <c r="F99" s="0" t="s">
         <v>7</v>
@@ -2726,16 +2722,16 @@
         <v>105</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>3.3501</v>
+        <v>3.42753</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>0.2472</v>
+        <v>0.4738</v>
       </c>
       <c r="D100" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E100" s="0" t="n">
-        <v>13.555</v>
+        <v>7.234</v>
       </c>
       <c r="F100" s="0" t="s">
         <v>7</v>
@@ -2746,16 +2742,16 @@
         <v>106</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>0.569944</v>
+        <v>0.65978</v>
       </c>
       <c r="C101" s="0" t="n">
-        <v>0.0537</v>
+        <v>0.0522</v>
       </c>
       <c r="D101" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E101" s="0" t="n">
-        <v>10.604</v>
+        <v>12.629</v>
       </c>
       <c r="F101" s="0" t="s">
         <v>7</v>
@@ -2766,16 +2762,16 @@
         <v>107</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>1.03974</v>
+        <v>0.95241</v>
       </c>
       <c r="C102" s="0" t="n">
-        <v>0.0593</v>
+        <v>0.075</v>
       </c>
       <c r="D102" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E102" s="0" t="n">
-        <v>17.539</v>
+        <v>12.705</v>
       </c>
       <c r="F102" s="0" t="s">
         <v>7</v>
@@ -2786,16 +2782,16 @@
         <v>108</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>1.225952</v>
+        <v>1.86038</v>
       </c>
       <c r="C103" s="0" t="n">
-        <v>0.0783</v>
+        <v>0.2622</v>
       </c>
       <c r="D103" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E103" s="0" t="n">
-        <v>15.649</v>
+        <v>7.096</v>
       </c>
       <c r="F103" s="0" t="s">
         <v>7</v>
@@ -2806,16 +2802,16 @@
         <v>109</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>4.483277</v>
+        <v>4.11701</v>
       </c>
       <c r="C104" s="0" t="n">
-        <v>0.3592</v>
+        <v>0.334</v>
       </c>
       <c r="D104" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E104" s="0" t="n">
-        <v>12.482</v>
+        <v>12.325</v>
       </c>
       <c r="F104" s="0" t="s">
         <v>7</v>
@@ -2826,16 +2822,16 @@
         <v>110</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>5.051946</v>
+        <v>4.35778</v>
       </c>
       <c r="C105" s="0" t="n">
-        <v>0.4357</v>
+        <v>0.3414</v>
       </c>
       <c r="D105" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E105" s="0" t="n">
-        <v>11.595</v>
+        <v>12.764</v>
       </c>
       <c r="F105" s="0" t="s">
         <v>7</v>
@@ -2846,16 +2842,16 @@
         <v>111</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>0.644357</v>
+        <v>0.57065</v>
       </c>
       <c r="C106" s="0" t="n">
-        <v>0.0854</v>
+        <v>0.0828</v>
       </c>
       <c r="D106" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E106" s="0" t="n">
-        <v>7.543</v>
+        <v>6.894</v>
       </c>
       <c r="F106" s="0" t="s">
         <v>7</v>
@@ -2866,16 +2862,16 @@
         <v>112</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>4.4831</v>
+        <v>4.322</v>
       </c>
       <c r="C107" s="0" t="n">
-        <v>0.3884</v>
+        <v>0.446</v>
       </c>
       <c r="D107" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E107" s="0" t="n">
-        <v>11.543</v>
+        <v>9.69</v>
       </c>
       <c r="F107" s="0" t="s">
         <v>7</v>
@@ -2886,16 +2882,16 @@
         <v>113</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>4.592384</v>
+        <v>5.71956</v>
       </c>
       <c r="C108" s="0" t="n">
-        <v>0.4082</v>
+        <v>1.024</v>
       </c>
       <c r="D108" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E108" s="0" t="n">
-        <v>11.25</v>
+        <v>5.586</v>
       </c>
       <c r="F108" s="0" t="s">
         <v>7</v>
@@ -2906,16 +2902,16 @@
         <v>114</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>2.801853</v>
+        <v>2.47528</v>
       </c>
       <c r="C109" s="0" t="n">
-        <v>0.164</v>
+        <v>0.1795</v>
       </c>
       <c r="D109" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E109" s="0" t="n">
-        <v>17.082</v>
+        <v>13.79</v>
       </c>
       <c r="F109" s="0" t="s">
         <v>7</v>
@@ -2926,16 +2922,16 @@
         <v>115</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>3.739445</v>
+        <v>3.34355</v>
       </c>
       <c r="C110" s="0" t="n">
-        <v>0.2625</v>
+        <v>0.1881</v>
       </c>
       <c r="D110" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E110" s="0" t="n">
-        <v>14.247</v>
+        <v>17.779</v>
       </c>
       <c r="F110" s="0" t="s">
         <v>7</v>
@@ -2946,16 +2942,16 @@
         <v>116</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>3.42821</v>
+        <v>2.63844</v>
       </c>
       <c r="C111" s="0" t="n">
-        <v>0.2911</v>
+        <v>0.1573</v>
       </c>
       <c r="D111" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E111" s="0" t="n">
-        <v>11.775</v>
+        <v>16.769</v>
       </c>
       <c r="F111" s="0" t="s">
         <v>7</v>
@@ -2966,16 +2962,16 @@
         <v>117</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>2.988236</v>
+        <v>3.47548</v>
       </c>
       <c r="C112" s="0" t="n">
-        <v>0.1722</v>
+        <v>0.2746</v>
       </c>
       <c r="D112" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E112" s="0" t="n">
-        <v>17.353</v>
+        <v>12.656</v>
       </c>
       <c r="F112" s="0" t="s">
         <v>7</v>
@@ -2986,16 +2982,16 @@
         <v>118</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>3.675083</v>
+        <v>3.4849</v>
       </c>
       <c r="C113" s="0" t="n">
-        <v>0.2469</v>
+        <v>0.4733</v>
       </c>
       <c r="D113" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E113" s="0" t="n">
-        <v>14.882</v>
+        <v>7.363</v>
       </c>
       <c r="F113" s="0" t="s">
         <v>7</v>
@@ -3006,19 +3002,19 @@
         <v>119</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>0.469795</v>
+        <v>0.29263</v>
       </c>
       <c r="C114" s="0" t="n">
-        <v>0.065</v>
+        <v>0.0832</v>
       </c>
       <c r="D114" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E114" s="0" t="n">
-        <v>7.224</v>
-      </c>
-      <c r="F114" s="0" t="s">
-        <v>7</v>
+        <v>3.519</v>
+      </c>
+      <c r="F114" s="0" t="n">
+        <v>0.0583</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3026,19 +3022,19 @@
         <v>120</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>0.656008</v>
+        <v>1.2006</v>
       </c>
       <c r="C115" s="0" t="n">
-        <v>0.0828</v>
+        <v>0.2646</v>
       </c>
       <c r="D115" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E115" s="0" t="n">
-        <v>7.925</v>
-      </c>
-      <c r="F115" s="0" t="s">
-        <v>7</v>
+        <v>4.537</v>
+      </c>
+      <c r="F115" s="0" t="n">
+        <v>0.0013</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3046,16 +3042,16 @@
         <v>121</v>
       </c>
       <c r="B116" s="0" t="n">
-        <v>3.913333</v>
+        <v>3.45723</v>
       </c>
       <c r="C116" s="0" t="n">
-        <v>0.3602</v>
+        <v>0.336</v>
       </c>
       <c r="D116" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E116" s="0" t="n">
-        <v>10.865</v>
+        <v>10.29</v>
       </c>
       <c r="F116" s="0" t="s">
         <v>7</v>
@@ -3066,16 +3062,16 @@
         <v>122</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>4.482002</v>
+        <v>3.698</v>
       </c>
       <c r="C117" s="0" t="n">
-        <v>0.4365</v>
+        <v>0.3433</v>
       </c>
       <c r="D117" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E117" s="0" t="n">
-        <v>10.267</v>
+        <v>10.772</v>
       </c>
       <c r="F117" s="0" t="s">
         <v>7</v>
@@ -3086,16 +3082,16 @@
         <v>123</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>0.074413</v>
+        <v>-0.08913</v>
       </c>
       <c r="C118" s="0" t="n">
-        <v>0.0895</v>
+        <v>0.0903</v>
       </c>
       <c r="D118" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E118" s="0" t="n">
-        <v>0.831</v>
+        <v>-0.987</v>
       </c>
       <c r="F118" s="0" t="n">
         <v>1</v>
@@ -3106,16 +3102,16 @@
         <v>124</v>
       </c>
       <c r="B119" s="0" t="n">
-        <v>3.913156</v>
+        <v>3.66223</v>
       </c>
       <c r="C119" s="0" t="n">
-        <v>0.3893</v>
+        <v>0.4475</v>
       </c>
       <c r="D119" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E119" s="0" t="n">
-        <v>10.052</v>
+        <v>8.184</v>
       </c>
       <c r="F119" s="0" t="s">
         <v>7</v>
@@ -3126,19 +3122,19 @@
         <v>125</v>
       </c>
       <c r="B120" s="0" t="n">
-        <v>4.02244</v>
+        <v>5.05978</v>
       </c>
       <c r="C120" s="0" t="n">
-        <v>0.4091</v>
+        <v>1.0246</v>
       </c>
       <c r="D120" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E120" s="0" t="n">
-        <v>9.833</v>
-      </c>
-      <c r="F120" s="0" t="s">
-        <v>7</v>
+        <v>4.938</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>0.0002</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3146,16 +3142,16 @@
         <v>126</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>2.231909</v>
+        <v>1.81551</v>
       </c>
       <c r="C121" s="0" t="n">
-        <v>0.1662</v>
+        <v>0.1831</v>
       </c>
       <c r="D121" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E121" s="0" t="n">
-        <v>13.43</v>
+        <v>9.917</v>
       </c>
       <c r="F121" s="0" t="s">
         <v>7</v>
@@ -3166,16 +3162,16 @@
         <v>127</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>3.1695</v>
+        <v>2.68377</v>
       </c>
       <c r="C122" s="0" t="n">
-        <v>0.2638</v>
+        <v>0.1915</v>
       </c>
       <c r="D122" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E122" s="0" t="n">
-        <v>12.013</v>
+        <v>14.017</v>
       </c>
       <c r="F122" s="0" t="s">
         <v>7</v>
@@ -3186,16 +3182,16 @@
         <v>128</v>
       </c>
       <c r="B123" s="0" t="n">
-        <v>2.858266</v>
+        <v>1.97866</v>
       </c>
       <c r="C123" s="0" t="n">
-        <v>0.2924</v>
+        <v>0.1614</v>
       </c>
       <c r="D123" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E123" s="0" t="n">
-        <v>9.776</v>
+        <v>12.259</v>
       </c>
       <c r="F123" s="0" t="s">
         <v>7</v>
@@ -3206,16 +3202,16 @@
         <v>129</v>
       </c>
       <c r="B124" s="0" t="n">
-        <v>2.418292</v>
+        <v>2.8157</v>
       </c>
       <c r="C124" s="0" t="n">
-        <v>0.1743</v>
+        <v>0.277</v>
       </c>
       <c r="D124" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E124" s="0" t="n">
-        <v>13.877</v>
+        <v>10.167</v>
       </c>
       <c r="F124" s="0" t="s">
         <v>7</v>
@@ -3226,16 +3222,16 @@
         <v>130</v>
       </c>
       <c r="B125" s="0" t="n">
-        <v>3.105139</v>
+        <v>2.82512</v>
       </c>
       <c r="C125" s="0" t="n">
-        <v>0.2484</v>
+        <v>0.4747</v>
       </c>
       <c r="D125" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E125" s="0" t="n">
-        <v>12.501</v>
+        <v>5.952</v>
       </c>
       <c r="F125" s="0" t="s">
         <v>7</v>
@@ -3246,19 +3242,19 @@
         <v>131</v>
       </c>
       <c r="B126" s="0" t="n">
-        <v>0.186212</v>
+        <v>0.90797</v>
       </c>
       <c r="C126" s="0" t="n">
-        <v>0.0865</v>
+        <v>0.27</v>
       </c>
       <c r="D126" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E126" s="0" t="n">
-        <v>2.153</v>
+        <v>3.363</v>
       </c>
       <c r="F126" s="0" t="n">
-        <v>0.8263</v>
+        <v>0.0931</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3266,16 +3262,16 @@
         <v>132</v>
       </c>
       <c r="B127" s="0" t="n">
-        <v>3.443537</v>
+        <v>3.1646</v>
       </c>
       <c r="C127" s="0" t="n">
-        <v>0.3611</v>
+        <v>0.3403</v>
       </c>
       <c r="D127" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E127" s="0" t="n">
-        <v>9.537</v>
+        <v>9.301</v>
       </c>
       <c r="F127" s="0" t="s">
         <v>7</v>
@@ -3286,16 +3282,16 @@
         <v>133</v>
       </c>
       <c r="B128" s="0" t="n">
-        <v>4.012206</v>
+        <v>3.40537</v>
       </c>
       <c r="C128" s="0" t="n">
-        <v>0.4373</v>
+        <v>0.3475</v>
       </c>
       <c r="D128" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E128" s="0" t="n">
-        <v>9.176</v>
+        <v>9.8</v>
       </c>
       <c r="F128" s="0" t="s">
         <v>7</v>
@@ -3306,19 +3302,19 @@
         <v>134</v>
       </c>
       <c r="B129" s="0" t="n">
-        <v>-0.395383</v>
+        <v>-0.38176</v>
       </c>
       <c r="C129" s="0" t="n">
-        <v>0.0929</v>
+        <v>0.1051</v>
       </c>
       <c r="D129" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E129" s="0" t="n">
-        <v>-4.254</v>
+        <v>-3.634</v>
       </c>
       <c r="F129" s="0" t="n">
-        <v>0.0042</v>
+        <v>0.0405</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3326,16 +3322,16 @@
         <v>135</v>
       </c>
       <c r="B130" s="0" t="n">
-        <v>3.44336</v>
+        <v>3.3696</v>
       </c>
       <c r="C130" s="0" t="n">
-        <v>0.3901</v>
+        <v>0.4507</v>
       </c>
       <c r="D130" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E130" s="0" t="n">
-        <v>8.827</v>
+        <v>7.476</v>
       </c>
       <c r="F130" s="0" t="s">
         <v>7</v>
@@ -3346,19 +3342,19 @@
         <v>136</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>3.552645</v>
+        <v>4.76715</v>
       </c>
       <c r="C131" s="0" t="n">
-        <v>0.4098</v>
+        <v>1.026</v>
       </c>
       <c r="D131" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E131" s="0" t="n">
-        <v>8.668</v>
-      </c>
-      <c r="F131" s="0" t="s">
-        <v>7</v>
+        <v>4.646</v>
+      </c>
+      <c r="F131" s="0" t="n">
+        <v>0.0008</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3366,16 +3362,16 @@
         <v>137</v>
       </c>
       <c r="B132" s="0" t="n">
-        <v>1.762114</v>
+        <v>1.52288</v>
       </c>
       <c r="C132" s="0" t="n">
-        <v>0.1681</v>
+        <v>0.1908</v>
       </c>
       <c r="D132" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E132" s="0" t="n">
-        <v>10.485</v>
+        <v>7.981</v>
       </c>
       <c r="F132" s="0" t="s">
         <v>7</v>
@@ -3386,16 +3382,16 @@
         <v>138</v>
       </c>
       <c r="B133" s="0" t="n">
-        <v>2.699705</v>
+        <v>2.39114</v>
       </c>
       <c r="C133" s="0" t="n">
-        <v>0.265</v>
+        <v>0.1989</v>
       </c>
       <c r="D133" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E133" s="0" t="n">
-        <v>10.187</v>
+        <v>12.024</v>
       </c>
       <c r="F133" s="0" t="s">
         <v>7</v>
@@ -3406,16 +3402,16 @@
         <v>139</v>
       </c>
       <c r="B134" s="0" t="n">
-        <v>2.38847</v>
+        <v>1.68603</v>
       </c>
       <c r="C134" s="0" t="n">
-        <v>0.2934</v>
+        <v>0.1701</v>
       </c>
       <c r="D134" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E134" s="0" t="n">
-        <v>8.14</v>
+        <v>9.911</v>
       </c>
       <c r="F134" s="0" t="s">
         <v>7</v>
@@ -3426,16 +3422,16 @@
         <v>140</v>
       </c>
       <c r="B135" s="0" t="n">
-        <v>1.948496</v>
+        <v>2.52308</v>
       </c>
       <c r="C135" s="0" t="n">
-        <v>0.176</v>
+        <v>0.2821</v>
       </c>
       <c r="D135" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E135" s="0" t="n">
-        <v>11.068</v>
+        <v>8.943</v>
       </c>
       <c r="F135" s="0" t="s">
         <v>7</v>
@@ -3446,16 +3442,16 @@
         <v>141</v>
       </c>
       <c r="B136" s="0" t="n">
-        <v>2.635343</v>
+        <v>2.53249</v>
       </c>
       <c r="C136" s="0" t="n">
-        <v>0.2496</v>
+        <v>0.4777</v>
       </c>
       <c r="D136" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E136" s="0" t="n">
-        <v>10.556</v>
+        <v>5.301</v>
       </c>
       <c r="F136" s="0" t="s">
         <v>7</v>
@@ -3466,16 +3462,16 @@
         <v>142</v>
       </c>
       <c r="B137" s="0" t="n">
-        <v>3.257325</v>
+        <v>2.25663</v>
       </c>
       <c r="C137" s="0" t="n">
-        <v>0.3647</v>
+        <v>0.4229</v>
       </c>
       <c r="D137" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E137" s="0" t="n">
-        <v>8.932</v>
+        <v>5.336</v>
       </c>
       <c r="F137" s="0" t="s">
         <v>7</v>
@@ -3486,16 +3482,16 @@
         <v>143</v>
       </c>
       <c r="B138" s="0" t="n">
-        <v>3.825994</v>
+        <v>2.4974</v>
       </c>
       <c r="C138" s="0" t="n">
-        <v>0.4402</v>
+        <v>0.4287</v>
       </c>
       <c r="D138" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E138" s="0" t="n">
-        <v>8.691</v>
+        <v>5.825</v>
       </c>
       <c r="F138" s="0" t="s">
         <v>7</v>
@@ -3506,19 +3502,19 @@
         <v>144</v>
       </c>
       <c r="B139" s="0" t="n">
-        <v>-0.581595</v>
+        <v>-1.28973</v>
       </c>
       <c r="C139" s="0" t="n">
-        <v>0.1061</v>
+        <v>0.2723</v>
       </c>
       <c r="D139" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E139" s="0" t="n">
-        <v>-5.48</v>
-      </c>
-      <c r="F139" s="0" t="s">
-        <v>7</v>
+        <v>-4.737</v>
+      </c>
+      <c r="F139" s="0" t="n">
+        <v>0.0005</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3526,19 +3522,19 @@
         <v>145</v>
       </c>
       <c r="B140" s="0" t="n">
-        <v>3.257148</v>
+        <v>2.46163</v>
       </c>
       <c r="C140" s="0" t="n">
-        <v>0.3934</v>
+        <v>0.5159</v>
       </c>
       <c r="D140" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E140" s="0" t="n">
-        <v>8.279</v>
-      </c>
-      <c r="F140" s="0" t="s">
-        <v>7</v>
+        <v>4.771</v>
+      </c>
+      <c r="F140" s="0" t="n">
+        <v>0.0005</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,19 +3542,19 @@
         <v>146</v>
       </c>
       <c r="B141" s="0" t="n">
-        <v>3.366432</v>
+        <v>3.85918</v>
       </c>
       <c r="C141" s="0" t="n">
-        <v>0.413</v>
+        <v>1.0563</v>
       </c>
       <c r="D141" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E141" s="0" t="n">
-        <v>8.151</v>
-      </c>
-      <c r="F141" s="0" t="s">
-        <v>7</v>
+        <v>3.653</v>
+      </c>
+      <c r="F141" s="0" t="n">
+        <v>0.038</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3566,19 +3562,19 @@
         <v>147</v>
       </c>
       <c r="B142" s="0" t="n">
-        <v>1.575901</v>
+        <v>0.6149</v>
       </c>
       <c r="C142" s="0" t="n">
-        <v>0.1757</v>
+        <v>0.3154</v>
       </c>
       <c r="D142" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E142" s="0" t="n">
-        <v>8.97</v>
-      </c>
-      <c r="F142" s="0" t="s">
-        <v>7</v>
+        <v>1.949</v>
+      </c>
+      <c r="F142" s="0" t="n">
+        <v>0.9201</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3586,19 +3582,19 @@
         <v>148</v>
       </c>
       <c r="B143" s="0" t="n">
-        <v>2.513493</v>
+        <v>1.48317</v>
       </c>
       <c r="C143" s="0" t="n">
-        <v>0.2699</v>
+        <v>0.3204</v>
       </c>
       <c r="D143" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E143" s="0" t="n">
-        <v>9.312</v>
-      </c>
-      <c r="F143" s="0" t="s">
-        <v>7</v>
+        <v>4.63</v>
+      </c>
+      <c r="F143" s="0" t="n">
+        <v>0.0009</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3606,19 +3602,19 @@
         <v>149</v>
       </c>
       <c r="B144" s="0" t="n">
-        <v>2.202258</v>
+        <v>0.77806</v>
       </c>
       <c r="C144" s="0" t="n">
-        <v>0.2979</v>
+        <v>0.3034</v>
       </c>
       <c r="D144" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E144" s="0" t="n">
-        <v>7.393</v>
-      </c>
-      <c r="F144" s="0" t="s">
-        <v>7</v>
+        <v>2.565</v>
+      </c>
+      <c r="F144" s="0" t="n">
+        <v>0.5344</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3626,19 +3622,19 @@
         <v>150</v>
       </c>
       <c r="B145" s="0" t="n">
-        <v>1.762284</v>
+        <v>1.6151</v>
       </c>
       <c r="C145" s="0" t="n">
-        <v>0.1833</v>
+        <v>0.3777</v>
       </c>
       <c r="D145" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E145" s="0" t="n">
-        <v>9.612</v>
-      </c>
-      <c r="F145" s="0" t="s">
-        <v>7</v>
+        <v>4.276</v>
+      </c>
+      <c r="F145" s="0" t="n">
+        <v>0.0038</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3646,19 +3642,19 @@
         <v>151</v>
       </c>
       <c r="B146" s="0" t="n">
-        <v>2.449131</v>
+        <v>1.62452</v>
       </c>
       <c r="C146" s="0" t="n">
-        <v>0.2548</v>
+        <v>0.5397</v>
       </c>
       <c r="D146" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E146" s="0" t="n">
-        <v>9.61</v>
-      </c>
-      <c r="F146" s="0" t="s">
-        <v>7</v>
+        <v>3.01</v>
+      </c>
+      <c r="F146" s="0" t="n">
+        <v>0.2316</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3666,16 +3662,16 @@
         <v>152</v>
       </c>
       <c r="B147" s="0" t="n">
-        <v>0.568669</v>
+        <v>0.24077</v>
       </c>
       <c r="C147" s="0" t="n">
-        <v>0.5587</v>
+        <v>0.4703</v>
       </c>
       <c r="D147" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E147" s="0" t="n">
-        <v>1.018</v>
+        <v>0.512</v>
       </c>
       <c r="F147" s="0" t="n">
         <v>1</v>
@@ -3686,16 +3682,16 @@
         <v>153</v>
       </c>
       <c r="B148" s="0" t="n">
-        <v>-3.83892</v>
+        <v>-3.54636</v>
       </c>
       <c r="C148" s="0" t="n">
-        <v>0.3663</v>
+        <v>0.3421</v>
       </c>
       <c r="D148" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E148" s="0" t="n">
-        <v>-10.482</v>
+        <v>-10.368</v>
       </c>
       <c r="F148" s="0" t="s">
         <v>7</v>
@@ -3706,16 +3702,16 @@
         <v>154</v>
       </c>
       <c r="B149" s="0" t="n">
-        <v>-0.000177</v>
+        <v>0.205</v>
       </c>
       <c r="C149" s="0" t="n">
-        <v>0.5206</v>
+        <v>0.549</v>
       </c>
       <c r="D149" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E149" s="0" t="n">
-        <v>0</v>
+        <v>0.373</v>
       </c>
       <c r="F149" s="0" t="n">
         <v>1</v>
@@ -3726,19 +3722,19 @@
         <v>155</v>
       </c>
       <c r="B150" s="0" t="n">
-        <v>0.109107</v>
+        <v>1.60255</v>
       </c>
       <c r="C150" s="0" t="n">
-        <v>0.5354</v>
+        <v>1.0745</v>
       </c>
       <c r="D150" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E150" s="0" t="n">
-        <v>0.204</v>
+        <v>1.491</v>
       </c>
       <c r="F150" s="0" t="n">
-        <v>1</v>
+        <v>0.9951</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3746,19 +3742,19 @@
         <v>156</v>
       </c>
       <c r="B151" s="0" t="n">
-        <v>-1.681424</v>
+        <v>-1.64173</v>
       </c>
       <c r="C151" s="0" t="n">
-        <v>0.391</v>
+        <v>0.3764</v>
       </c>
       <c r="D151" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E151" s="0" t="n">
-        <v>-4.3</v>
+        <v>-4.361</v>
       </c>
       <c r="F151" s="0" t="n">
-        <v>0.0035</v>
+        <v>0.0027</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3766,19 +3762,19 @@
         <v>157</v>
       </c>
       <c r="B152" s="0" t="n">
-        <v>-0.743832</v>
+        <v>-0.77346</v>
       </c>
       <c r="C152" s="0" t="n">
-        <v>0.4379</v>
+        <v>0.3764</v>
       </c>
       <c r="D152" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E152" s="0" t="n">
-        <v>-1.699</v>
+        <v>-2.055</v>
       </c>
       <c r="F152" s="0" t="n">
-        <v>0.9786</v>
+        <v>0.8771</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3786,19 +3782,19 @@
         <v>158</v>
       </c>
       <c r="B153" s="0" t="n">
-        <v>-1.055067</v>
+        <v>-1.47857</v>
       </c>
       <c r="C153" s="0" t="n">
-        <v>0.4532</v>
+        <v>0.3661</v>
       </c>
       <c r="D153" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E153" s="0" t="n">
-        <v>-2.328</v>
+        <v>-4.039</v>
       </c>
       <c r="F153" s="0" t="n">
-        <v>0.7137</v>
+        <v>0.0097</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3806,19 +3802,19 @@
         <v>159</v>
       </c>
       <c r="B154" s="0" t="n">
-        <v>-1.495041</v>
+        <v>-0.64153</v>
       </c>
       <c r="C154" s="0" t="n">
-        <v>0.3942</v>
+        <v>0.4279</v>
       </c>
       <c r="D154" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E154" s="0" t="n">
-        <v>-3.792</v>
+        <v>-1.499</v>
       </c>
       <c r="F154" s="0" t="n">
-        <v>0.0237</v>
+        <v>0.9948</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3826,19 +3822,19 @@
         <v>160</v>
       </c>
       <c r="B155" s="0" t="n">
-        <v>-0.808194</v>
+        <v>-0.63211</v>
       </c>
       <c r="C155" s="0" t="n">
-        <v>0.4295</v>
+        <v>0.5735</v>
       </c>
       <c r="D155" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E155" s="0" t="n">
-        <v>-1.882</v>
+        <v>-1.102</v>
       </c>
       <c r="F155" s="0" t="n">
-        <v>0.9415</v>
+        <v>0.9999</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3846,16 +3842,16 @@
         <v>161</v>
       </c>
       <c r="B156" s="0" t="n">
-        <v>-4.407589</v>
+        <v>-3.78713</v>
       </c>
       <c r="C156" s="0" t="n">
-        <v>0.4416</v>
+        <v>0.3493</v>
       </c>
       <c r="D156" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E156" s="0" t="n">
-        <v>-9.982</v>
+        <v>-10.843</v>
       </c>
       <c r="F156" s="0" t="s">
         <v>7</v>
@@ -3866,16 +3862,16 @@
         <v>162</v>
       </c>
       <c r="B157" s="0" t="n">
-        <v>-0.568846</v>
+        <v>-0.03577</v>
       </c>
       <c r="C157" s="0" t="n">
-        <v>0.577</v>
+        <v>0.5533</v>
       </c>
       <c r="D157" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E157" s="0" t="n">
-        <v>-0.986</v>
+        <v>-0.065</v>
       </c>
       <c r="F157" s="0" t="n">
         <v>1</v>
@@ -3886,19 +3882,19 @@
         <v>163</v>
       </c>
       <c r="B158" s="0" t="n">
-        <v>-0.459562</v>
+        <v>1.36178</v>
       </c>
       <c r="C158" s="0" t="n">
-        <v>0.5903</v>
+        <v>1.0767</v>
       </c>
       <c r="D158" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E158" s="0" t="n">
-        <v>-0.778</v>
+        <v>1.265</v>
       </c>
       <c r="F158" s="0" t="n">
-        <v>1</v>
+        <v>0.9994</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3906,19 +3902,19 @@
         <v>164</v>
       </c>
       <c r="B159" s="0" t="n">
-        <v>-2.250093</v>
+        <v>-1.88249</v>
       </c>
       <c r="C159" s="0" t="n">
-        <v>0.4625</v>
+        <v>0.3829</v>
       </c>
       <c r="D159" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E159" s="0" t="n">
-        <v>-4.865</v>
+        <v>-4.916</v>
       </c>
       <c r="F159" s="0" t="n">
-        <v>0.0003</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3926,19 +3922,19 @@
         <v>165</v>
       </c>
       <c r="B160" s="0" t="n">
-        <v>-1.312501</v>
+        <v>-1.01423</v>
       </c>
       <c r="C160" s="0" t="n">
-        <v>0.5032</v>
+        <v>0.3828</v>
       </c>
       <c r="D160" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E160" s="0" t="n">
-        <v>-2.608</v>
+        <v>-2.65</v>
       </c>
       <c r="F160" s="0" t="n">
-        <v>0.5006</v>
+        <v>0.469</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3946,19 +3942,19 @@
         <v>166</v>
       </c>
       <c r="B161" s="0" t="n">
-        <v>-1.623736</v>
+        <v>-1.71934</v>
       </c>
       <c r="C161" s="0" t="n">
-        <v>0.5169</v>
+        <v>0.3727</v>
       </c>
       <c r="D161" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E161" s="0" t="n">
-        <v>-3.141</v>
+        <v>-4.613</v>
       </c>
       <c r="F161" s="0" t="n">
-        <v>0.169</v>
+        <v>0.0009</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3966,19 +3962,19 @@
         <v>167</v>
       </c>
       <c r="B162" s="0" t="n">
-        <v>-2.06371</v>
+        <v>-0.88229</v>
       </c>
       <c r="C162" s="0" t="n">
-        <v>0.4652</v>
+        <v>0.4336</v>
       </c>
       <c r="D162" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E162" s="0" t="n">
-        <v>-4.436</v>
+        <v>-2.035</v>
       </c>
       <c r="F162" s="0" t="n">
-        <v>0.002</v>
+        <v>0.8862</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3986,19 +3982,19 @@
         <v>168</v>
       </c>
       <c r="B163" s="0" t="n">
-        <v>-1.376863</v>
+        <v>-0.87288</v>
       </c>
       <c r="C163" s="0" t="n">
-        <v>0.4958</v>
+        <v>0.5777</v>
       </c>
       <c r="D163" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E163" s="0" t="n">
-        <v>-2.777</v>
+        <v>-1.511</v>
       </c>
       <c r="F163" s="0" t="n">
-        <v>0.3758</v>
+        <v>0.9943</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4006,16 +4002,16 @@
         <v>169</v>
       </c>
       <c r="B164" s="0" t="n">
-        <v>3.838743</v>
+        <v>3.75136</v>
       </c>
       <c r="C164" s="0" t="n">
-        <v>0.3949</v>
+        <v>0.4521</v>
       </c>
       <c r="D164" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E164" s="0" t="n">
-        <v>9.721</v>
+        <v>8.298</v>
       </c>
       <c r="F164" s="0" t="s">
         <v>7</v>
@@ -4026,19 +4022,19 @@
         <v>170</v>
       </c>
       <c r="B165" s="0" t="n">
-        <v>3.948027</v>
+        <v>5.14891</v>
       </c>
       <c r="C165" s="0" t="n">
-        <v>0.4144</v>
+        <v>1.0266</v>
       </c>
       <c r="D165" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E165" s="0" t="n">
-        <v>9.526</v>
-      </c>
-      <c r="F165" s="0" t="s">
-        <v>7</v>
+        <v>5.015</v>
+      </c>
+      <c r="F165" s="0" t="n">
+        <v>0.0001</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4046,16 +4042,16 @@
         <v>171</v>
       </c>
       <c r="B166" s="0" t="n">
-        <v>2.157496</v>
+        <v>1.90464</v>
       </c>
       <c r="C166" s="0" t="n">
-        <v>0.179</v>
+        <v>0.194</v>
       </c>
       <c r="D166" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E166" s="0" t="n">
-        <v>12.055</v>
+        <v>9.817</v>
       </c>
       <c r="F166" s="0" t="s">
         <v>7</v>
@@ -4066,16 +4062,16 @@
         <v>172</v>
       </c>
       <c r="B167" s="0" t="n">
-        <v>3.095088</v>
+        <v>2.7729</v>
       </c>
       <c r="C167" s="0" t="n">
-        <v>0.2721</v>
+        <v>0.2019</v>
       </c>
       <c r="D167" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E167" s="0" t="n">
-        <v>11.376</v>
+        <v>13.731</v>
       </c>
       <c r="F167" s="0" t="s">
         <v>7</v>
@@ -4086,16 +4082,16 @@
         <v>173</v>
       </c>
       <c r="B168" s="0" t="n">
-        <v>2.783853</v>
+        <v>2.06779</v>
       </c>
       <c r="C168" s="0" t="n">
-        <v>0.2998</v>
+        <v>0.1737</v>
       </c>
       <c r="D168" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E168" s="0" t="n">
-        <v>9.285</v>
+        <v>11.904</v>
       </c>
       <c r="F168" s="0" t="s">
         <v>7</v>
@@ -4106,16 +4102,16 @@
         <v>174</v>
       </c>
       <c r="B169" s="0" t="n">
-        <v>2.343879</v>
+        <v>2.90484</v>
       </c>
       <c r="C169" s="0" t="n">
-        <v>0.1865</v>
+        <v>0.2843</v>
       </c>
       <c r="D169" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E169" s="0" t="n">
-        <v>12.569</v>
+        <v>10.218</v>
       </c>
       <c r="F169" s="0" t="s">
         <v>7</v>
@@ -4126,16 +4122,16 @@
         <v>175</v>
       </c>
       <c r="B170" s="0" t="n">
-        <v>3.030726</v>
+        <v>2.91425</v>
       </c>
       <c r="C170" s="0" t="n">
-        <v>0.2571</v>
+        <v>0.479</v>
       </c>
       <c r="D170" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E170" s="0" t="n">
-        <v>11.787</v>
+        <v>6.084</v>
       </c>
       <c r="F170" s="0" t="s">
         <v>7</v>
@@ -4146,19 +4142,19 @@
         <v>176</v>
       </c>
       <c r="B171" s="0" t="n">
-        <v>0.109284</v>
+        <v>1.39755</v>
       </c>
       <c r="C171" s="0" t="n">
-        <v>0.5539</v>
+        <v>1.1136</v>
       </c>
       <c r="D171" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E171" s="0" t="n">
-        <v>0.197</v>
+        <v>1.255</v>
       </c>
       <c r="F171" s="0" t="n">
-        <v>1</v>
+        <v>0.9995</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4166,19 +4162,19 @@
         <v>177</v>
       </c>
       <c r="B172" s="0" t="n">
-        <v>-1.681247</v>
+        <v>-1.84672</v>
       </c>
       <c r="C172" s="0" t="n">
-        <v>0.4178</v>
+        <v>0.4783</v>
       </c>
       <c r="D172" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E172" s="0" t="n">
-        <v>-4.024</v>
+        <v>-3.861</v>
       </c>
       <c r="F172" s="0" t="n">
-        <v>0.0102</v>
+        <v>0.0186</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4186,19 +4182,19 @@
         <v>178</v>
       </c>
       <c r="B173" s="0" t="n">
-        <v>-0.743655</v>
+        <v>-0.97846</v>
       </c>
       <c r="C173" s="0" t="n">
-        <v>0.4611</v>
+        <v>0.4768</v>
       </c>
       <c r="D173" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E173" s="0" t="n">
-        <v>-1.613</v>
+        <v>-2.052</v>
       </c>
       <c r="F173" s="0" t="n">
-        <v>0.9878</v>
+        <v>0.8784</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4206,19 +4202,19 @@
         <v>179</v>
       </c>
       <c r="B174" s="0" t="n">
-        <v>-1.05489</v>
+        <v>-1.68357</v>
       </c>
       <c r="C174" s="0" t="n">
-        <v>0.4751</v>
+        <v>0.4701</v>
       </c>
       <c r="D174" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E174" s="0" t="n">
-        <v>-2.22</v>
+        <v>-3.582</v>
       </c>
       <c r="F174" s="0" t="n">
-        <v>0.7863</v>
+        <v>0.0479</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4226,19 +4222,19 @@
         <v>180</v>
       </c>
       <c r="B175" s="0" t="n">
-        <v>-1.494864</v>
+        <v>-0.84652</v>
       </c>
       <c r="C175" s="0" t="n">
-        <v>0.4207</v>
+        <v>0.519</v>
       </c>
       <c r="D175" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E175" s="0" t="n">
-        <v>-3.553</v>
+        <v>-1.631</v>
       </c>
       <c r="F175" s="0" t="n">
-        <v>0.0524</v>
+        <v>0.9862</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4246,19 +4242,19 @@
         <v>181</v>
       </c>
       <c r="B176" s="0" t="n">
-        <v>-0.808017</v>
+        <v>-0.83711</v>
       </c>
       <c r="C176" s="0" t="n">
-        <v>0.4533</v>
+        <v>0.6435</v>
       </c>
       <c r="D176" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E176" s="0" t="n">
-        <v>-1.782</v>
+        <v>-1.301</v>
       </c>
       <c r="F176" s="0" t="n">
-        <v>0.965</v>
+        <v>0.9992</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4266,19 +4262,19 @@
         <v>182</v>
       </c>
       <c r="B177" s="0" t="n">
-        <v>-1.790531</v>
+        <v>-3.24427</v>
       </c>
       <c r="C177" s="0" t="n">
-        <v>0.4362</v>
+        <v>1.0386</v>
       </c>
       <c r="D177" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E177" s="0" t="n">
-        <v>-4.105</v>
+        <v>-3.124</v>
       </c>
       <c r="F177" s="0" t="n">
-        <v>0.0075</v>
+        <v>0.1767</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4286,19 +4282,19 @@
         <v>183</v>
       </c>
       <c r="B178" s="0" t="n">
-        <v>-0.85294</v>
+        <v>-2.37601</v>
       </c>
       <c r="C178" s="0" t="n">
-        <v>0.4778</v>
+        <v>1.039</v>
       </c>
       <c r="D178" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E178" s="0" t="n">
-        <v>-1.785</v>
+        <v>-2.287</v>
       </c>
       <c r="F178" s="0" t="n">
-        <v>0.9644</v>
+        <v>0.7425</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4306,19 +4302,19 @@
         <v>184</v>
       </c>
       <c r="B179" s="0" t="n">
-        <v>-1.164174</v>
+        <v>-3.08112</v>
       </c>
       <c r="C179" s="0" t="n">
-        <v>0.4912</v>
+        <v>1.035</v>
       </c>
       <c r="D179" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E179" s="0" t="n">
-        <v>-2.37</v>
+        <v>-2.977</v>
       </c>
       <c r="F179" s="0" t="n">
-        <v>0.6832</v>
+        <v>0.2496</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4326,19 +4322,19 @@
         <v>185</v>
       </c>
       <c r="B180" s="0" t="n">
-        <v>-1.604148</v>
+        <v>-2.24407</v>
       </c>
       <c r="C180" s="0" t="n">
-        <v>0.439</v>
+        <v>1.0586</v>
       </c>
       <c r="D180" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E180" s="0" t="n">
-        <v>-3.654</v>
+        <v>-2.12</v>
       </c>
       <c r="F180" s="0" t="n">
-        <v>0.0379</v>
+        <v>0.8447</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4346,19 +4342,19 @@
         <v>186</v>
       </c>
       <c r="B181" s="0" t="n">
-        <v>-0.917301</v>
+        <v>-2.23466</v>
       </c>
       <c r="C181" s="0" t="n">
-        <v>0.4703</v>
+        <v>1.1257</v>
       </c>
       <c r="D181" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E181" s="0" t="n">
-        <v>-1.951</v>
+        <v>-1.985</v>
       </c>
       <c r="F181" s="0" t="n">
-        <v>0.9196</v>
+        <v>0.9068</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4366,19 +4362,19 @@
         <v>187</v>
       </c>
       <c r="B182" s="0" t="n">
-        <v>0.937591</v>
+        <v>0.86826</v>
       </c>
       <c r="C182" s="0" t="n">
-        <v>0.305</v>
+        <v>0.2562</v>
       </c>
       <c r="D182" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E182" s="0" t="n">
-        <v>3.074</v>
+        <v>3.388</v>
       </c>
       <c r="F182" s="0" t="n">
-        <v>0.1992</v>
+        <v>0.0864</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4386,19 +4382,19 @@
         <v>188</v>
       </c>
       <c r="B183" s="0" t="n">
-        <v>0.626357</v>
+        <v>0.16315</v>
       </c>
       <c r="C183" s="0" t="n">
-        <v>0.3294</v>
+        <v>0.2354</v>
       </c>
       <c r="D183" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E183" s="0" t="n">
-        <v>1.901</v>
+        <v>0.693</v>
       </c>
       <c r="F183" s="0" t="n">
-        <v>0.9358</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4406,19 +4402,19 @@
         <v>189</v>
       </c>
       <c r="B184" s="0" t="n">
-        <v>0.186383</v>
+        <v>1.0002</v>
       </c>
       <c r="C184" s="0" t="n">
-        <v>0.2328</v>
+        <v>0.3254</v>
       </c>
       <c r="D184" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E184" s="0" t="n">
-        <v>0.8</v>
+        <v>3.074</v>
       </c>
       <c r="F184" s="0" t="n">
-        <v>1</v>
+        <v>0.1995</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4426,19 +4422,19 @@
         <v>190</v>
       </c>
       <c r="B185" s="0" t="n">
-        <v>0.87323</v>
+        <v>1.00961</v>
       </c>
       <c r="C185" s="0" t="n">
-        <v>0.2919</v>
+        <v>0.5041</v>
       </c>
       <c r="D185" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E185" s="0" t="n">
-        <v>2.992</v>
+        <v>2.003</v>
       </c>
       <c r="F185" s="0" t="n">
-        <v>0.2415</v>
+        <v>0.8999</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4446,19 +4442,19 @@
         <v>191</v>
       </c>
       <c r="B186" s="0" t="n">
-        <v>-0.311235</v>
+        <v>-0.70511</v>
       </c>
       <c r="C186" s="0" t="n">
-        <v>0.3832</v>
+        <v>0.2409</v>
       </c>
       <c r="D186" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E186" s="0" t="n">
-        <v>-0.812</v>
+        <v>-2.927</v>
       </c>
       <c r="F186" s="0" t="n">
-        <v>1</v>
+        <v>0.2784</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4466,19 +4462,19 @@
         <v>192</v>
       </c>
       <c r="B187" s="0" t="n">
-        <v>-0.751209</v>
+        <v>0.13193</v>
       </c>
       <c r="C187" s="0" t="n">
-        <v>0.3092</v>
+        <v>0.328</v>
       </c>
       <c r="D187" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E187" s="0" t="n">
-        <v>-2.43</v>
+        <v>0.402</v>
       </c>
       <c r="F187" s="0" t="n">
-        <v>0.6386</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4486,16 +4482,16 @@
         <v>193</v>
       </c>
       <c r="B188" s="0" t="n">
-        <v>-0.064362</v>
+        <v>0.14135</v>
       </c>
       <c r="C188" s="0" t="n">
-        <v>0.3539</v>
+        <v>0.5042</v>
       </c>
       <c r="D188" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E188" s="0" t="n">
-        <v>-0.182</v>
+        <v>0.28</v>
       </c>
       <c r="F188" s="0" t="n">
         <v>1</v>
@@ -4506,19 +4502,19 @@
         <v>194</v>
       </c>
       <c r="B189" s="0" t="n">
-        <v>-0.439974</v>
+        <v>0.83705</v>
       </c>
       <c r="C189" s="0" t="n">
-        <v>0.3332</v>
+        <v>0.3135</v>
       </c>
       <c r="D189" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E189" s="0" t="n">
-        <v>-1.321</v>
+        <v>2.67</v>
       </c>
       <c r="F189" s="0" t="n">
-        <v>0.999</v>
+        <v>0.454</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4526,19 +4522,19 @@
         <v>195</v>
       </c>
       <c r="B190" s="0" t="n">
-        <v>0.246873</v>
+        <v>0.84646</v>
       </c>
       <c r="C190" s="0" t="n">
-        <v>0.3737</v>
+        <v>0.4964</v>
       </c>
       <c r="D190" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E190" s="0" t="n">
-        <v>0.661</v>
+        <v>1.705</v>
       </c>
       <c r="F190" s="0" t="n">
-        <v>1</v>
+        <v>0.9777</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4546,19 +4542,19 @@
         <v>196</v>
       </c>
       <c r="B191" s="0" t="n">
-        <v>0.686847</v>
+        <v>0.00941</v>
       </c>
       <c r="C191" s="0" t="n">
-        <v>0.2963</v>
+        <v>0.5437</v>
       </c>
       <c r="D191" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E191" s="0" t="n">
-        <v>2.318</v>
+        <v>0.017</v>
       </c>
       <c r="F191" s="0" t="n">
-        <v>0.7208</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4579,8 +4575,8 @@
   </sheetPr>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4613,16 +4609,16 @@
         <v>11</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>-0.605961</v>
+        <v>-0.64418</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0.0602</v>
+        <v>0.0596</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>-10.07</v>
+        <v>-10.804</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>7</v>
@@ -4633,16 +4629,16 @@
         <v>16</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>3.552333</v>
+        <v>3.41546</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.3611</v>
+        <v>0.3365</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>9.839</v>
+        <v>10.151</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>7</v>
@@ -4653,16 +4649,16 @@
         <v>21</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1.870909</v>
+        <v>1.77374</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.1681</v>
+        <v>0.1839</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>11.131</v>
+        <v>9.643</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>7</v>
@@ -4673,19 +4669,19 @@
         <v>30</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>-0.416395</v>
+        <v>-0.16565</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.0496</v>
+        <v>0.0408</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>-8.394</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>7</v>
+        <v>-4.064</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.0088</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4693,16 +4689,16 @@
         <v>35</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>4.635551</v>
+        <v>4.19213</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.436</v>
+        <v>0.3417</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>10.631</v>
+        <v>12.267</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>7</v>
@@ -4713,16 +4709,16 @@
         <v>40</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>3.32305</v>
+        <v>3.1779</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0.263</v>
+        <v>0.1887</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>12.634</v>
+        <v>16.845</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>7</v>
@@ -4733,16 +4729,16 @@
         <v>48</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0.298749</v>
+        <v>0.71788</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>0.0553</v>
+        <v>0.0506</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>5.401</v>
+        <v>14.196</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>7</v>
@@ -4753,19 +4749,19 @@
         <v>53</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0.373162</v>
+        <v>0.62875</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0.0864</v>
+        <v>0.0817</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>4.318</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>0.0032</v>
+        <v>7.693</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4773,16 +4769,16 @@
         <v>58</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>3.157015</v>
+        <v>2.69654</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>0.2914</v>
+        <v>0.1568</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>10.833</v>
+        <v>17.198</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>7</v>
@@ -4793,16 +4789,16 @@
         <v>65</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.907514</v>
+        <v>0.58383</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>0.0584</v>
+        <v>0.0931</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>15.549</v>
+        <v>6.273</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>7</v>
@@ -4813,16 +4809,16 @@
         <v>70</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>4.350874</v>
+        <v>3.95343</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>0.3882</v>
+        <v>0.4494</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>11.207</v>
+        <v>8.797</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>7</v>
@@ -4833,16 +4829,16 @@
         <v>75</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>2.85601</v>
+        <v>3.1069</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>0.1719</v>
+        <v>0.2801</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>16.616</v>
+        <v>11.093</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>7</v>
@@ -4853,39 +4849,39 @@
         <v>81</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>0.723544</v>
+        <v>1.54309</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>0.0809</v>
+        <v>0.3108</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>8.942</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+        <v>4.965</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.0002</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="1" t="n">
-        <v>4.089977</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>0.4087</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>394</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>10.007</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>7</v>
+      <c r="B15" s="0" t="n">
+        <v>5.40227</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1.0375</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>394</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>5.207</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.0001</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4893,16 +4889,16 @@
         <v>91</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>3.172675</v>
+        <v>3.16761</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>0.2478</v>
+        <v>0.5019</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>12.805</v>
+        <v>6.312</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>7</v>
@@ -4913,16 +4909,16 @@
         <v>96</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>4.158294</v>
+        <v>4.05964</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>0.3593</v>
+        <v>0.3348</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>11.572</v>
+        <v>12.125</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>7</v>
@@ -4933,16 +4929,16 @@
         <v>101</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>2.47687</v>
+        <v>2.41792</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0.1643</v>
+        <v>0.1809</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>15.072</v>
+        <v>13.365</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>7</v>
@@ -4953,16 +4949,16 @@
         <v>110</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>5.051946</v>
+        <v>4.35778</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>0.4357</v>
+        <v>0.3414</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>11.595</v>
+        <v>12.764</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>7</v>
@@ -4973,16 +4969,16 @@
         <v>115</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>3.739445</v>
+        <v>3.34355</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>0.2625</v>
+        <v>0.1881</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>14.247</v>
+        <v>17.779</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>7</v>
@@ -4993,16 +4989,16 @@
         <v>123</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>0.074413</v>
+        <v>-0.08913</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>0.0895</v>
+        <v>0.0903</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>0.831</v>
+        <v>-0.987</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>1</v>
@@ -5013,16 +5009,16 @@
         <v>128</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>2.858266</v>
+        <v>1.97866</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>0.2924</v>
+        <v>0.1614</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>9.776</v>
+        <v>12.259</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>7</v>
@@ -5033,16 +5029,16 @@
         <v>135</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>3.44336</v>
+        <v>3.3696</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>0.3901</v>
+        <v>0.4507</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>8.827</v>
+        <v>7.476</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>7</v>
@@ -5053,16 +5049,16 @@
         <v>140</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>1.948496</v>
+        <v>2.52308</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>0.176</v>
+        <v>0.2821</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>11.068</v>
+        <v>8.943</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>7</v>
@@ -5073,19 +5069,19 @@
         <v>146</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>3.366432</v>
+        <v>3.85918</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>0.413</v>
+        <v>1.0563</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>8.151</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>7</v>
+        <v>3.653</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>0.038</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5093,19 +5089,19 @@
         <v>151</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>2.449131</v>
+        <v>1.62452</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>0.2548</v>
+        <v>0.5397</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>9.61</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>7</v>
+        <v>3.01</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0.2316</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5113,19 +5109,19 @@
         <v>156</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>-1.681424</v>
+        <v>-1.64173</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>0.391</v>
+        <v>0.3764</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>-4.3</v>
+        <v>-4.361</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>0.0035</v>
+        <v>0.0027</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5133,19 +5129,19 @@
         <v>165</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>-1.312501</v>
+        <v>-1.01423</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>0.5032</v>
+        <v>0.3828</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>-2.608</v>
+        <v>-2.65</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>0.5006</v>
+        <v>0.469</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5153,16 +5149,16 @@
         <v>173</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>2.783853</v>
+        <v>2.06779</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>0.2998</v>
+        <v>0.1737</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>9.285</v>
+        <v>11.904</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>7</v>
@@ -5173,19 +5169,19 @@
         <v>180</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>-1.494864</v>
+        <v>-0.84652</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>0.4207</v>
+        <v>0.519</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>-3.553</v>
+        <v>-1.631</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>0.0524</v>
+        <v>0.9862</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5193,19 +5189,19 @@
         <v>186</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>-0.917301</v>
+        <v>-2.23466</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>0.4703</v>
+        <v>1.1257</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>394</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>-1.951</v>
+        <v>-1.985</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>0.9196</v>
+        <v>0.9068</v>
       </c>
     </row>
   </sheetData>
@@ -5226,7 +5222,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>